<commit_message>
modified:   ServidorDentista.xlsx modified:   server.js
</commit_message>
<xml_diff>
--- a/ServidorDentista.xlsx
+++ b/ServidorDentista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mamut\Desktop\PWebDent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114E909B-AAD1-4712-AB46-A6D21745DF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84020E5B-6EB8-47D1-8BE9-D4683F150B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>10:00</t>
+  </si>
+  <si>
+    <t>Antonio Hernandez</t>
+  </si>
+  <si>
+    <t>antonio.hernandezmm@gmail.com</t>
+  </si>
+  <si>
+    <t>95212026</t>
+  </si>
+  <si>
+    <t>+54 (11) 24097694</t>
+  </si>
+  <si>
+    <t>2025-02-13</t>
+  </si>
+  <si>
+    <t>02:18</t>
   </si>
 </sst>
 </file>
@@ -407,18 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.8984375" customWidth="1"/>
-    <col min="2" max="2" width="19.09765625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="2" max="2" width="35.796875" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -461,10 +476,30 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>